<commit_message>
update in yaml, minor fixes in positions counter script, data overview
</commit_message>
<xml_diff>
--- a/training_run_information.xlsx
+++ b/training_run_information.xlsx
@@ -8,24 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0_Repos\lczero-training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE22383-8145-45BA-AE40-DE54E3269D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D712C9-B105-4B2B-8D77-06657AD95510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -43,6 +57,33 @@
   </si>
   <si>
     <t>Number of positions</t>
+  </si>
+  <si>
+    <t>training-run1--20230505-0217</t>
+  </si>
+  <si>
+    <t>training-run1--20230415-1317</t>
+  </si>
+  <si>
+    <t>training-run1--20250209-1017</t>
+  </si>
+  <si>
+    <t>Total number of positions</t>
+  </si>
+  <si>
+    <t>training-run1--20230415-1417</t>
+  </si>
+  <si>
+    <t>training-run1--20230505-0317</t>
+  </si>
+  <si>
+    <t>training-run1--20230505-0817</t>
+  </si>
+  <si>
+    <t>training-run1--20230505-0917</t>
+  </si>
+  <si>
+    <t>training-run2--20210605-0517</t>
   </si>
 </sst>
 </file>
@@ -375,21 +416,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,22 +444,178 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>94183</v>
+      </c>
+      <c r="D2">
+        <v>10368107</v>
+      </c>
+      <c r="E2">
+        <f>D2</f>
+        <v>10368107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>36521</v>
+      </c>
+      <c r="D3">
+        <v>4045389</v>
+      </c>
+      <c r="E3">
+        <f>E2+D3</f>
+        <v>14413496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>82910</v>
+      </c>
+      <c r="D4">
+        <v>9020629</v>
+      </c>
+      <c r="E4">
+        <f>E3+D4</f>
+        <v>23434125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>28343</v>
+      </c>
+      <c r="D5">
+        <v>3122029</v>
+      </c>
+      <c r="E5">
+        <f>E4+D5</f>
+        <v>26556154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>36203</v>
+      </c>
+      <c r="D6">
+        <v>4012237</v>
+      </c>
+      <c r="E6">
+        <f>E5+D6</f>
+        <v>30568391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>18083</v>
+      </c>
+      <c r="D7">
+        <v>1978914</v>
+      </c>
+      <c r="E7">
+        <f>E6+D7</f>
+        <v>32547305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
         <v>35423</v>
       </c>
-      <c r="D2">
+      <c r="D8">
         <v>3894864</v>
       </c>
+      <c r="E8">
+        <f>E7+D8</f>
+        <v>36442169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>19443</v>
+      </c>
+      <c r="D9">
+        <v>2142829</v>
+      </c>
+      <c r="E9">
+        <f>E8+D9</f>
+        <v>38584998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>33992</v>
+      </c>
+      <c r="D10">
+        <v>3688005</v>
+      </c>
+      <c r="E10">
+        <f>E9+D10</f>
+        <v>42273003</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- data_scraper.py to get list of datasets - text file containing 50 largest files - table documentation number of positions - position counter script - yaml config for 6M model
</commit_message>
<xml_diff>
--- a/training_run_information.xlsx
+++ b/training_run_information.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0_Repos\lczero-training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D712C9-B105-4B2B-8D77-06657AD95510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B20EB38-D976-4D2E-BE82-5224873AEC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Valid sets" sheetId="1" r:id="rId1"/>
+    <sheet name="Sets with corrupted data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Valid sets'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -84,6 +85,48 @@
   </si>
   <si>
     <t>training-run2--20210605-0517</t>
+  </si>
+  <si>
+    <t>training-run1--20210605-0516</t>
+  </si>
+  <si>
+    <t>training-run3--20210605-0521</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210314-1134</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210923-1917</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210618-0354</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210603-1203</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210924-0917</t>
+  </si>
+  <si>
+    <t>Averaged positions per chunk</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210815-1418</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210924-0617</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210923-2017</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210923-2117</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210923-2317</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210923-2217</t>
   </si>
 </sst>
 </file>
@@ -138,7 +181,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -416,22 +459,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7265625" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.6328125" customWidth="1"/>
+    <col min="7" max="7" width="33.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,176 +492,445 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2">
-        <v>94183</v>
+        <v>2662</v>
       </c>
       <c r="D2">
-        <v>10368107</v>
+        <v>278008</v>
       </c>
       <c r="E2">
         <f>D2</f>
+        <v>278008</v>
+      </c>
+      <c r="G2">
+        <f>SUM(D2:D18)/SUM(C2:C18)</f>
+        <v>108.91356665929507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>94183</v>
+      </c>
+      <c r="D3">
         <v>10368107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>36521</v>
-      </c>
-      <c r="D3">
-        <v>4045389</v>
       </c>
       <c r="E3">
         <f>E2+D3</f>
-        <v>14413496</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>10646115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>82910</v>
+        <v>36521</v>
       </c>
       <c r="D4">
-        <v>9020629</v>
+        <v>4045389</v>
       </c>
       <c r="E4">
         <f>E3+D4</f>
-        <v>23434125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>14691504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>28343</v>
+        <v>82910</v>
       </c>
       <c r="D5">
-        <v>3122029</v>
+        <v>9020629</v>
       </c>
       <c r="E5">
         <f>E4+D5</f>
-        <v>26556154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>23712133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>36203</v>
+        <v>28343</v>
       </c>
       <c r="D6">
-        <v>4012237</v>
+        <v>3122029</v>
       </c>
       <c r="E6">
         <f>E5+D6</f>
-        <v>30568391</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>26834162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7">
-        <v>18083</v>
+        <v>36203</v>
       </c>
       <c r="D7">
-        <v>1978914</v>
+        <v>4012237</v>
       </c>
       <c r="E7">
         <f>E6+D7</f>
-        <v>32547305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>30846399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8">
-        <v>35423</v>
+        <v>18083</v>
       </c>
       <c r="D8">
-        <v>3894864</v>
+        <v>1978914</v>
       </c>
       <c r="E8">
         <f>E7+D8</f>
-        <v>36442169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>32825313</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9">
-        <v>19443</v>
+        <v>35423</v>
       </c>
       <c r="D9">
-        <v>2142829</v>
+        <v>3894864</v>
       </c>
       <c r="E9">
         <f>E8+D9</f>
-        <v>38584998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+        <v>36720177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10">
-        <v>33992</v>
+        <v>19443</v>
       </c>
       <c r="D10">
-        <v>3688005</v>
+        <v>2142829</v>
       </c>
       <c r="E10">
         <f>E9+D10</f>
-        <v>42273003</v>
+        <v>38863006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>33992</v>
+      </c>
+      <c r="D11">
+        <v>3688005</v>
+      </c>
+      <c r="E11">
+        <f>E10+D11</f>
+        <v>42551011</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>7690</v>
+      </c>
+      <c r="D12">
+        <v>849932</v>
+      </c>
+      <c r="E12">
+        <f>E11+D12</f>
+        <v>43400943</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>80538</v>
+      </c>
+      <c r="D13">
+        <v>7525057</v>
+      </c>
+      <c r="E13">
+        <f>E12+D13</f>
+        <v>50926000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>368438</v>
+      </c>
+      <c r="D14">
+        <v>40517339</v>
+      </c>
+      <c r="E14">
+        <f>E13+D14</f>
+        <v>91443339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>326093</v>
+      </c>
+      <c r="D15">
+        <v>36007682</v>
+      </c>
+      <c r="E15">
+        <f>E14+D15</f>
+        <v>127451021</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>326188</v>
+      </c>
+      <c r="D16">
+        <v>35718012</v>
+      </c>
+      <c r="E16">
+        <f>E15+D16</f>
+        <v>163169033</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>331177</v>
+      </c>
+      <c r="D17">
+        <v>35989481</v>
+      </c>
+      <c r="E17">
+        <f>E16+D17</f>
+        <v>199158514</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>310952</v>
+      </c>
+      <c r="D18">
+        <v>33790070</v>
+      </c>
+      <c r="E18">
+        <f>E17+D18</f>
+        <v>232948584</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>304853</v>
+      </c>
+      <c r="D19">
+        <v>33141797</v>
+      </c>
+      <c r="E19">
+        <f>E18+D19</f>
+        <v>266090381</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>302375</v>
+      </c>
+      <c r="D20">
+        <v>32875805</v>
+      </c>
+      <c r="E20">
+        <f>E19+D20</f>
+        <v>298966186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21">
+        <v>303109</v>
+      </c>
+      <c r="D21">
+        <v>32958247</v>
+      </c>
+      <c r="E21">
+        <f>E20+D21</f>
+        <v>331924433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>315833</v>
+      </c>
+      <c r="D22">
+        <v>34336028</v>
+      </c>
+      <c r="E22">
+        <f>E21+D22</f>
+        <v>366260461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>600000</v>
+      </c>
+      <c r="D23">
+        <v>65263374</v>
+      </c>
+      <c r="E23">
+        <f>E22+D23</f>
+        <v>431523835</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19733B62-E14D-41B3-9563-11A6F5B089B6}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates in yaml and doc sheet
</commit_message>
<xml_diff>
--- a/training_run_information.xlsx
+++ b/training_run_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0_Repos\lczero-training\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B20EB38-D976-4D2E-BE82-5224873AEC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36759CC1-5CAE-4312-B566-6D0986288FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8890" yWindow="2080" windowWidth="24550" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid sets" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>name</t>
   </si>
@@ -127,6 +127,18 @@
   </si>
   <si>
     <t>training-run3-test75-20210923-2217</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210924-0517
+training-run3-test75-20210924-0717
+training-run3-test75-20210924-0817</t>
+  </si>
+  <si>
+    <t>training-run3-test75-20210924-0117
+training-run3-test75-20210924-0217</t>
+  </si>
+  <si>
+    <t>Total number of chunks</t>
   </si>
 </sst>
 </file>
@@ -176,9 +188,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -459,15 +474,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.08984375" customWidth="1"/>
     <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.7265625" customWidth="1"/>
@@ -492,6 +507,9 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
@@ -513,9 +531,13 @@
         <f>D2</f>
         <v>278008</v>
       </c>
+      <c r="F2">
+        <f>C2</f>
+        <v>2662</v>
+      </c>
       <c r="G2">
-        <f>SUM(D2:D18)/SUM(C2:C18)</f>
-        <v>108.91356665929507</v>
+        <f>SUM(D2:D25)/SUM(C2:C25)</f>
+        <v>108.80899788448355</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -532,8 +554,12 @@
         <v>10368107</v>
       </c>
       <c r="E3">
-        <f>E2+D3</f>
+        <f t="shared" ref="E3:E25" si="0">E2+D3</f>
         <v>10646115</v>
+      </c>
+      <c r="F3">
+        <f>F2+C3</f>
+        <v>96845</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -550,8 +576,12 @@
         <v>4045389</v>
       </c>
       <c r="E4">
-        <f>E3+D4</f>
+        <f t="shared" si="0"/>
         <v>14691504</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F25" si="1">F3+C4</f>
+        <v>133366</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -568,8 +598,12 @@
         <v>9020629</v>
       </c>
       <c r="E5">
-        <f>E4+D5</f>
+        <f t="shared" si="0"/>
         <v>23712133</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>216276</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -586,8 +620,12 @@
         <v>3122029</v>
       </c>
       <c r="E6">
-        <f>E5+D6</f>
+        <f t="shared" si="0"/>
         <v>26834162</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>244619</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -604,8 +642,12 @@
         <v>4012237</v>
       </c>
       <c r="E7">
-        <f>E6+D7</f>
+        <f t="shared" si="0"/>
         <v>30846399</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>280822</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -622,8 +664,12 @@
         <v>1978914</v>
       </c>
       <c r="E8">
-        <f>E7+D8</f>
+        <f t="shared" si="0"/>
         <v>32825313</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>298905</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -640,8 +686,12 @@
         <v>3894864</v>
       </c>
       <c r="E9">
-        <f>E8+D9</f>
+        <f t="shared" si="0"/>
         <v>36720177</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>334328</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -658,8 +708,12 @@
         <v>2142829</v>
       </c>
       <c r="E10">
-        <f>E9+D10</f>
+        <f t="shared" si="0"/>
         <v>38863006</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>353771</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -676,8 +730,12 @@
         <v>3688005</v>
       </c>
       <c r="E11">
-        <f>E10+D11</f>
+        <f t="shared" si="0"/>
         <v>42551011</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>387763</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -694,8 +752,12 @@
         <v>849932</v>
       </c>
       <c r="E12">
-        <f>E11+D12</f>
+        <f t="shared" si="0"/>
         <v>43400943</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>395453</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -712,8 +774,12 @@
         <v>7525057</v>
       </c>
       <c r="E13">
-        <f>E12+D13</f>
+        <f t="shared" si="0"/>
         <v>50926000</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>475991</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -730,8 +796,12 @@
         <v>40517339</v>
       </c>
       <c r="E14">
-        <f>E13+D14</f>
+        <f t="shared" si="0"/>
         <v>91443339</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>844429</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -748,8 +818,12 @@
         <v>36007682</v>
       </c>
       <c r="E15">
-        <f>E14+D15</f>
+        <f t="shared" si="0"/>
         <v>127451021</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>1170522</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -766,11 +840,15 @@
         <v>35718012</v>
       </c>
       <c r="E16">
-        <f>E15+D16</f>
+        <f t="shared" si="0"/>
         <v>163169033</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>1496710</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -784,11 +862,15 @@
         <v>35989481</v>
       </c>
       <c r="E17">
-        <f>E16+D17</f>
+        <f t="shared" si="0"/>
         <v>199158514</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>1827887</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -802,11 +884,15 @@
         <v>33790070</v>
       </c>
       <c r="E18">
-        <f>E17+D18</f>
+        <f t="shared" si="0"/>
         <v>232948584</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>2138839</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -820,11 +906,15 @@
         <v>33141797</v>
       </c>
       <c r="E19">
-        <f>E18+D19</f>
+        <f t="shared" si="0"/>
         <v>266090381</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>2443692</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -838,11 +928,15 @@
         <v>32875805</v>
       </c>
       <c r="E20">
-        <f>E19+D20</f>
+        <f t="shared" si="0"/>
         <v>298966186</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2746067</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -856,49 +950,105 @@
         <v>32958247</v>
       </c>
       <c r="E21">
-        <f>E20+D21</f>
+        <f t="shared" si="0"/>
         <v>331924433</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>3049176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>600000</v>
+      </c>
+      <c r="D22">
+        <v>65242480</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>397166913</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>3649176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23">
+        <v>903632</v>
+      </c>
+      <c r="D23">
+        <v>98271032</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>495437945</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>4552808</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24">
         <v>315833</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>34336028</v>
       </c>
-      <c r="E22">
-        <f>E21+D22</f>
-        <v>366260461</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>529773973</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>4868641</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23">
+      <c r="B25" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25">
         <v>600000</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>65263374</v>
       </c>
-      <c r="E23">
-        <f>E22+D23</f>
-        <v>431523835</v>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>595037347</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>5468641</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E23">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>